<commit_message>
add wells and GIS
</commit_message>
<xml_diff>
--- a/Assignments/Week 3 - ATES/GIS/background_wells.xlsx
+++ b/Assignments/Week 3 - ATES/GIS/background_wells.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\Studie TUD\Msc\Year 6\Q2 Subsurface storage for energy, water and climate\Project\design-ASR-CEGM2006\Assignments\Week 3 - ATES\GIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B14F70-8F14-42A7-9616-B859673C4353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0877BA0F-B9E0-4D88-9F10-9F3F222DA7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>